<commit_message>
added new pdf files required during submission
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -1,37 +1,96 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\Projects\microsoft-movie-analysis\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Genre</t>
+  </si>
+  <si>
+    <t>Votes</t>
+  </si>
+  <si>
+    <t>AverageVotes</t>
+  </si>
+  <si>
+    <t>AverageRating</t>
+  </si>
+  <si>
+    <t>Action,Adventure,Sci-Fi</t>
+  </si>
+  <si>
+    <t>Action,Drama,Sci-Fi</t>
+  </si>
+  <si>
+    <t>Action,Adventure,Comedy</t>
+  </si>
+  <si>
+    <t>Action,Adventure,Fantasy</t>
+  </si>
+  <si>
+    <t>Adventure,Drama,Sci-Fi</t>
+  </si>
+  <si>
+    <t>Biography,Crime,Drama</t>
+  </si>
+  <si>
+    <t>Action,Thriller</t>
+  </si>
+  <si>
+    <t>Adventure,Drama,Fantasy</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,94 +105,46 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -421,234 +432,210 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Year</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Genre</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Votes</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>AverageVotes</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>AverageRating</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>2019</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Action,Adventure,Sci-Fi</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
         <v>737360</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>368680</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>7.9</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2018</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Action,Adventure,Sci-Fi</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
         <v>670926</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>670926</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>8.5</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>2017</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Action,Drama,Sci-Fi</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
         <v>560270</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>560270</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>8.1</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>2016</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Action,Adventure,Comedy</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
         <v>820847</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>820847</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5">
         <v>8</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="n">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>2015</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Action,Adventure,Fantasy</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
         <v>784780</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>784780</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6">
         <v>8</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="n">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>2014</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Adventure,Drama,Sci-Fi</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
         <v>1299334</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7">
         <v>1299334</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7">
         <v>8.6</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="n">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>2013</v>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Biography,Crime,Drama</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
         <v>1035358</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8">
         <v>1035358</v>
       </c>
-      <c r="E8" t="n">
-        <v>8.199999999999999</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
+      <c r="E8">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>2012</v>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Action,Thriller</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
         <v>1387769</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9">
         <v>1387769</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9">
         <v>8.4</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="n">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>2011</v>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Adventure,Drama,Fantasy</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10">
         <v>691835</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D10">
         <v>691835</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10">
         <v>8.1</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="n">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>2010</v>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Action,Adventure,Sci-Fi</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11">
         <v>1841066</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D11">
         <v>1841066</v>
       </c>
-      <c r="E11" t="n">
-        <v>8.800000000000001</v>
+      <c r="E11">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="2">
+        <f>SUM(C2:C11)</f>
+        <v>9829545</v>
       </c>
     </row>
   </sheetData>

</xml_diff>